<commit_message>
Added dstat handling scripts
</commit_message>
<xml_diff>
--- a/processing/final/benchmark_memcached/benchmark_memcached.xlsx
+++ b/processing/final/benchmark_memcached/benchmark_memcached.xlsx
@@ -233,8 +233,8 @@
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
-      <c:lineChart>
-        <c:grouping val="standard"/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
         <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
@@ -252,7 +252,19 @@
             <a:effectLst/>
           </c:spPr>
           <c:marker>
-            <c:symbol val="none"/>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
           </c:marker>
           <c:errBars>
             <c:errDir val="y"/>
@@ -342,7 +354,7 @@
               <a:effectLst/>
             </c:spPr>
           </c:errBars>
-          <c:cat>
+          <c:xVal>
             <c:numRef>
               <c:f>data!$D$5:$D$22</c:f>
               <c:numCache>
@@ -404,8 +416,8 @@
                 </c:pt>
               </c:numCache>
             </c:numRef>
-          </c:cat>
-          <c:val>
+          </c:xVal>
+          <c:yVal>
             <c:numRef>
               <c:f>data!$E$5:$E$13</c:f>
               <c:numCache>
@@ -440,7 +452,7 @@
                 </c:pt>
               </c:numCache>
             </c:numRef>
-          </c:val>
+          </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
         <c:ser>
@@ -459,7 +471,19 @@
             <a:effectLst/>
           </c:spPr>
           <c:marker>
-            <c:symbol val="none"/>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
           </c:marker>
           <c:errBars>
             <c:errDir val="y"/>
@@ -549,7 +573,7 @@
               <a:effectLst/>
             </c:spPr>
           </c:errBars>
-          <c:cat>
+          <c:xVal>
             <c:numRef>
               <c:f>data!$D$5:$D$22</c:f>
               <c:numCache>
@@ -611,8 +635,8 @@
                 </c:pt>
               </c:numCache>
             </c:numRef>
-          </c:cat>
-          <c:val>
+          </c:xVal>
+          <c:yVal>
             <c:numRef>
               <c:f>data!$E$14:$E$22</c:f>
               <c:numCache>
@@ -647,7 +671,7 @@
                 </c:pt>
               </c:numCache>
             </c:numRef>
-          </c:val>
+          </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
         <c:dLbls>
@@ -658,12 +682,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:smooth val="0"/>
-        <c:axId val="1006902512"/>
-        <c:axId val="1006905072"/>
-      </c:lineChart>
-      <c:catAx>
-        <c:axId val="1006902512"/>
+        <c:axId val="-509207056"/>
+        <c:axId val="-699654736"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="-509207056"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -767,15 +790,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1006905072"/>
+        <c:crossAx val="-699654736"/>
         <c:crosses val="autoZero"/>
-        <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
-        <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="0"/>
-      </c:catAx>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
       <c:valAx>
-        <c:axId val="1006905072"/>
+        <c:axId val="-699654736"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -886,9 +906,9 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1006902512"/>
+        <c:crossAx val="-509207056"/>
         <c:crosses val="autoZero"/>
-        <c:crossBetween val="between"/>
+        <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:spPr>
         <a:noFill/>
@@ -1054,8 +1074,8 @@
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
-      <c:lineChart>
-        <c:grouping val="standard"/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
         <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
@@ -1073,7 +1093,19 @@
             <a:effectLst/>
           </c:spPr>
           <c:marker>
-            <c:symbol val="none"/>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
           </c:marker>
           <c:errBars>
             <c:errDir val="y"/>
@@ -1163,7 +1195,7 @@
               <a:effectLst/>
             </c:spPr>
           </c:errBars>
-          <c:cat>
+          <c:xVal>
             <c:numRef>
               <c:f>data!$D$5:$D$22</c:f>
               <c:numCache>
@@ -1225,8 +1257,8 @@
                 </c:pt>
               </c:numCache>
             </c:numRef>
-          </c:cat>
-          <c:val>
+          </c:xVal>
+          <c:yVal>
             <c:numRef>
               <c:f>data!$G$5:$G$13</c:f>
               <c:numCache>
@@ -1261,7 +1293,7 @@
                 </c:pt>
               </c:numCache>
             </c:numRef>
-          </c:val>
+          </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
         <c:ser>
@@ -1280,7 +1312,19 @@
             <a:effectLst/>
           </c:spPr>
           <c:marker>
-            <c:symbol val="none"/>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
           </c:marker>
           <c:errBars>
             <c:errDir val="y"/>
@@ -1370,7 +1414,7 @@
               <a:effectLst/>
             </c:spPr>
           </c:errBars>
-          <c:cat>
+          <c:xVal>
             <c:numRef>
               <c:f>data!$D$5:$D$22</c:f>
               <c:numCache>
@@ -1432,8 +1476,8 @@
                 </c:pt>
               </c:numCache>
             </c:numRef>
-          </c:cat>
-          <c:val>
+          </c:xVal>
+          <c:yVal>
             <c:numRef>
               <c:f>data!$G$14:$G$22</c:f>
               <c:numCache>
@@ -1468,7 +1512,7 @@
                 </c:pt>
               </c:numCache>
             </c:numRef>
-          </c:val>
+          </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
         <c:dLbls>
@@ -1479,12 +1523,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:smooth val="0"/>
-        <c:axId val="1006776320"/>
-        <c:axId val="1006778864"/>
-      </c:lineChart>
-      <c:catAx>
-        <c:axId val="1006776320"/>
+        <c:axId val="-510310928"/>
+        <c:axId val="-699606704"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="-510310928"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1588,15 +1631,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1006778864"/>
+        <c:crossAx val="-699606704"/>
         <c:crosses val="autoZero"/>
-        <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
-        <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="0"/>
-      </c:catAx>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
       <c:valAx>
-        <c:axId val="1006778864"/>
+        <c:axId val="-699606704"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1702,9 +1742,9 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1006776320"/>
+        <c:crossAx val="-510310928"/>
         <c:crosses val="autoZero"/>
-        <c:crossBetween val="between"/>
+        <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:spPr>
         <a:noFill/>
@@ -3731,8 +3771,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:X22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R36" sqref="R36"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="Q45" sqref="Q45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>